<commit_message>
Attempted Implementation for Mini Batching
</commit_message>
<xml_diff>
--- a/ELEUV0214_SM22_0214L2_30.xlsx
+++ b/ELEUV0214_SM22_0214L2_30.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="21">
   <si>
     <t>Tagname</t>
   </si>
@@ -23,6 +23,60 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120Current Average</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120Voltage Phase AN</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120Frequency</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120DMD</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120Current Phase A</t>
+  </si>
+  <si>
+    <t>UVA/Data/Buildings/0214/ac_Buildings0214MetersELEUV0214_SM31_0214L2_61_120Voltage L to N Average</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:15:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:20:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:25:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:30:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:35:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:40:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:45:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:50:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 07:55:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 08:05:00</t>
+  </si>
+  <si>
+    <t>2020-09-20 08:10:00</t>
   </si>
 </sst>
 </file>
@@ -380,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,6 +449,944 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0.32854128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>120.04922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>60.00719100000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.025006296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0.32854128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>60.01218000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>120.02985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0.31243297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>0.034641307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.44874468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>60.02920899999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0.42488703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>120.07967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0.29678628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>0.030971667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>0.32855275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>60.019505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>0.31796584</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>119.89315</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>119.97749</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>0.024864011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>0.4156951</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>59.99313000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>0.4156951</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>119.87875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>119.87875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>0.031664301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29">
+        <v>59.984051</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>0.05116464900000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>0.65200549</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>119.92761</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>119.92761</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>0.65200549</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0.31821519</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>120.15597</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>119.94876</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>0.35241956</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>59.993908</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>0.025441322</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>120.11074</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>0.026074907</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43">
+        <v>0.33554524</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44">
+        <v>120.02058</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>0.30651543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>60.01041800000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <v>120.46729</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48">
+        <v>0.0465906</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>0.58445209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50">
+        <v>0.38045797</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <v>120.4466</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52">
+        <v>60.015697</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53">
+        <v>119.95953</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54">
+        <v>0.024717616</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55">
+        <v>60.02498199999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <v>0.32390133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57">
+        <v>0.31395879</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58">
+        <v>120.15672</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59">
+        <v>120.0101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60">
+        <v>0.05264922599999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61">
+        <v>120.0101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62">
+        <v>0.63969535</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63">
+        <v>0.63969535</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64">
+        <v>120.29406</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>0.023294078</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66">
+        <v>0.30281147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67">
+        <v>0.30281147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68">
+        <v>120.29406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>